<commit_message>
Updated Modified Datasets Extraction
</commit_message>
<xml_diff>
--- a/media_output_labels.xlsx
+++ b/media_output_labels.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D112"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,16 +461,16 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="3">
@@ -479,12 +479,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -497,16 +497,16 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="5">
@@ -515,16 +515,16 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D1-Texting</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D1-Texting</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="6">
@@ -533,16 +533,16 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -551,12 +551,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -569,16 +569,16 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.95</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="9">
@@ -587,12 +587,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -605,12 +605,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D1-Texting</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D1-Texting</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -623,16 +623,16 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="12">
@@ -641,16 +641,16 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="13">
@@ -668,7 +668,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.91</v>
+        <v>0.9399999999999999</v>
       </c>
     </row>
     <row r="14">
@@ -677,16 +677,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0.98</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="15">
@@ -695,12 +695,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>D1-Texting</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>D1-Texting</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.97</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="17">
@@ -731,16 +731,16 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="18">
@@ -749,16 +749,16 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="19">
@@ -767,16 +767,16 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0.95</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="20">
@@ -785,16 +785,16 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="21">
@@ -803,16 +803,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>0.97</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="22">
@@ -821,16 +821,16 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>background</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="23">
@@ -839,16 +839,16 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>0.99</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="24">
@@ -857,16 +857,16 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0.84</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="25">
@@ -875,16 +875,16 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="26">
@@ -893,16 +893,16 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D1-Texting</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D1-Texting</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>0.99</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="27">
@@ -911,16 +911,16 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0.96</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="28">
@@ -929,16 +929,16 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0.88</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="29">
@@ -947,12 +947,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -965,12 +965,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -988,11 +988,11 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0.97</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="32">
@@ -1010,7 +1010,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0.97</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="33">
@@ -1019,16 +1019,16 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0.93</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="34">
@@ -1037,16 +1037,16 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0.79</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="35">
@@ -1055,16 +1055,16 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0.97</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -1073,12 +1073,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -1091,16 +1091,16 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0.99</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="38">
@@ -1109,12 +1109,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1127,12 +1127,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1154,7 +1154,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.99</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="41">
@@ -1163,16 +1163,16 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.96</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1181,16 +1181,16 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -1199,16 +1199,16 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.72</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -1217,16 +1217,16 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="45">
@@ -1235,16 +1235,16 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0.99</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="46">
@@ -1262,7 +1262,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0.98</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -1271,16 +1271,16 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0.99</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="48">
@@ -1289,16 +1289,16 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="49">
@@ -1316,7 +1316,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="50">
@@ -1325,16 +1325,16 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.99</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="51">
@@ -1343,12 +1343,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -1370,7 +1370,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>1</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="53">
@@ -1379,12 +1379,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D1-Texting</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D1-Texting</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -1397,12 +1397,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="D54" t="n">
@@ -1415,16 +1415,16 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>1</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="56">
@@ -1433,12 +1433,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -1451,16 +1451,16 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>0.97</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -1469,16 +1469,16 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>background</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="D58" t="n">
-        <v>1</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="59">
@@ -1487,16 +1487,16 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>background</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>0.79</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -1505,16 +1505,16 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="61">
@@ -1523,12 +1523,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -1541,16 +1541,16 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="D62" t="n">
-        <v>1</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="63">
@@ -1559,16 +1559,16 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="64">
@@ -1577,16 +1577,16 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>0.99</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="65">
@@ -1595,12 +1595,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D1-Texting</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D1-Texting</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -1613,16 +1613,16 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>0.95</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="67">
@@ -1631,16 +1631,16 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="68">
@@ -1649,16 +1649,16 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>D1-Texting</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>D1-Texting</t>
         </is>
       </c>
       <c r="D68" t="n">
-        <v>0.97</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="69">
@@ -1667,16 +1667,16 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>0.95</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="70">
@@ -1685,16 +1685,16 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>0.87</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="71">
@@ -1703,39 +1703,39 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>0.95</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>0.62</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
@@ -1748,21 +1748,21 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="D74" t="n">
@@ -1771,34 +1771,34 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>0.98</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -1807,61 +1807,61 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>background</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>0.66</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="D79" t="n">
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
@@ -1879,88 +1879,88 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D2-Calling</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D4-Reach-Behind</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D1-Texting</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D1-Texting</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>1</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>0.95</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="D85" t="n">
@@ -1969,16 +1969,16 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>D4-Reach-Behind</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="D86" t="n">
@@ -1987,52 +1987,52 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>0.97</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D3-Drinking</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>0.99</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D1-Texting</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>D0-Hand-on-Wheel</t>
+          <t>D1-Texting</t>
         </is>
       </c>
       <c r="D89" t="n">
@@ -2041,7 +2041,7 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
@@ -2054,30 +2054,30 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>0.99</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>D2-Calling</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
@@ -2090,21 +2090,21 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>D3-Drinking</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="D93" t="n">
@@ -2113,344 +2113,20 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>D1-Texting</t>
+          <t>D0-Hand-on-Wheel</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="n">
-        <v>93</v>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>D2-Calling</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>D2-Calling</t>
-        </is>
-      </c>
-      <c r="D95" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="n">
-        <v>94</v>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>D4-Reach-Behind</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>D4-Reach-Behind</t>
-        </is>
-      </c>
-      <c r="D96" t="n">
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n">
-        <v>95</v>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>D3-Drinking</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>D3-Drinking</t>
-        </is>
-      </c>
-      <c r="D97" t="n">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="n">
-        <v>96</v>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>D2-Calling</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>D2-Calling</t>
-        </is>
-      </c>
-      <c r="D98" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="n">
-        <v>97</v>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>D0-Hand-on-Wheel</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>D0-Hand-on-Wheel</t>
-        </is>
-      </c>
-      <c r="D99" t="n">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="n">
-        <v>98</v>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>D0-Hand-on-Wheel</t>
-        </is>
-      </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>D0-Hand-on-Wheel</t>
-        </is>
-      </c>
-      <c r="D100" t="n">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="n">
-        <v>99</v>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>D0-Hand-on-Wheel</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>D0-Hand-on-Wheel</t>
-        </is>
-      </c>
-      <c r="D101" t="n">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="n">
-        <v>100</v>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>D2-Calling</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>D2-Calling</t>
-        </is>
-      </c>
-      <c r="D102" t="n">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="n">
-        <v>101</v>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>D2-Calling</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>D2-Calling</t>
-        </is>
-      </c>
-      <c r="D103" t="n">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="n">
-        <v>102</v>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>D1-Texting</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>D0-Hand-on-Wheel</t>
-        </is>
-      </c>
-      <c r="D104" t="n">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="n">
-        <v>103</v>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>D1-Texting</t>
-        </is>
-      </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>D1-Texting</t>
-        </is>
-      </c>
-      <c r="D105" t="n">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="n">
-        <v>104</v>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>D1-Texting</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>D1-Texting</t>
-        </is>
-      </c>
-      <c r="D106" t="n">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="n">
-        <v>105</v>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>D3-Drinking</t>
-        </is>
-      </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>D3-Drinking</t>
-        </is>
-      </c>
-      <c r="D107" t="n">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="n">
-        <v>106</v>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>D1-Texting</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>D1-Texting</t>
-        </is>
-      </c>
-      <c r="D108" t="n">
-        <v>0.97</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="n">
-        <v>107</v>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>D3-Drinking</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>D3-Drinking</t>
-        </is>
-      </c>
-      <c r="D109" t="n">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="n">
-        <v>108</v>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>D4-Reach-Behind</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>D4-Reach-Behind</t>
-        </is>
-      </c>
-      <c r="D110" t="n">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="n">
-        <v>109</v>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>D0-Hand-on-Wheel</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>D0-Hand-on-Wheel</t>
-        </is>
-      </c>
-      <c r="D111" t="n">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="n">
-        <v>110</v>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>D4-Reach-Behind</t>
-        </is>
-      </c>
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>D4-Reach-Behind</t>
-        </is>
-      </c>
-      <c r="D112" t="n">
-        <v>0.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>